<commit_message>
2021/12/17 Media and Wiring
- Fixed issue with patch panels.
- Terminated wires, probably terribly, but at least have the lengths and wrap done. Will re-crimp properly later (before using the wires).
- Finished up the `T Slot Wire Anchor` design.
- Tested panel mount--will need to be moved backwards.
- Added a wire guide for the right `XY Joint` to keep the harness elevated.
- Redesigned wire panel mounts to sit further back, leaving more room for exiting wire.
- Added a folder for test GCODE and a basic movement test file, though it needs...testing.
- Modified Z limit switches to lower them 6mm.
- Discovered issue with BLTouch mount after attaching cable ties. Will probably try and move mount position forward a few mm.
</commit_message>
<xml_diff>
--- a/Docs/Connectors.xlsx
+++ b/Docs/Connectors.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEA5517-EA9B-4BC0-A354-90E9FD8279DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91143369-5505-4124-B5FE-F8637260D940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
+    <workbookView xWindow="24288" yWindow="1296" windowWidth="26832" windowHeight="14196" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Connector</t>
   </si>
@@ -57,12 +58,6 @@
     <t>TH0</t>
   </si>
   <si>
-    <t>F0</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
     <t>Part Cooling Fan</t>
   </si>
   <si>
@@ -81,30 +76,18 @@
     <t>Auto Bed Leveling</t>
   </si>
   <si>
-    <t>E0</t>
-  </si>
-  <si>
     <t>Extruder Stepper</t>
   </si>
   <si>
     <t>E0 (MOT4 on Octopus)</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>X Limit Switch</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Y Limit Switch</t>
   </si>
   <si>
-    <t>Z1</t>
-  </si>
-  <si>
     <t>Left Z Limit Switch</t>
   </si>
   <si>
@@ -117,9 +100,6 @@
     <t>Z-STOP/Z-MIN</t>
   </si>
   <si>
-    <t>Z2</t>
-  </si>
-  <si>
     <t>Right Z Limit Switch</t>
   </si>
   <si>
@@ -153,49 +133,97 @@
     <t>Bed Power</t>
   </si>
   <si>
-    <t>THB</t>
-  </si>
-  <si>
     <t>Bed Thermistor</t>
   </si>
   <si>
     <t>External Connectors</t>
   </si>
   <si>
-    <t>MOTA</t>
-  </si>
-  <si>
     <t>Alpha Stepper</t>
   </si>
   <si>
     <t>X-MOT</t>
   </si>
   <si>
-    <t>MOTB</t>
-  </si>
-  <si>
     <t>Beta Stepper</t>
   </si>
   <si>
     <t>Y-MOT</t>
   </si>
   <si>
-    <t>MOTZ1</t>
-  </si>
-  <si>
     <t>Z1 Stepper</t>
   </si>
   <si>
     <t>Z-MOT</t>
   </si>
   <si>
-    <t>MOTZ2</t>
-  </si>
-  <si>
     <t>Z2 Stepper</t>
   </si>
   <si>
     <t>E1-MOT</t>
+  </si>
+  <si>
+    <t>SX</t>
+  </si>
+  <si>
+    <t>SY</t>
+  </si>
+  <si>
+    <t>SZ1</t>
+  </si>
+  <si>
+    <t>SZ2</t>
+  </si>
+  <si>
+    <t>HE</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>BED</t>
+  </si>
+  <si>
+    <t>MZ2</t>
+  </si>
+  <si>
+    <t>MZ1</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Chamber Thermistor</t>
+  </si>
+  <si>
+    <t>FC1</t>
+  </si>
+  <si>
+    <t>FC2</t>
+  </si>
+  <si>
+    <t>Chamber Exhaust</t>
+  </si>
+  <si>
+    <t>Chamber Filtration</t>
+  </si>
+  <si>
+    <t>FH1</t>
+  </si>
+  <si>
+    <t>FH2</t>
   </si>
 </sst>
 </file>
@@ -260,8 +288,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}" name="Table1" displayName="Table1" ref="A1:C21" totalsRowShown="0">
-  <autoFilter ref="A1:C21" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}" name="Table1" displayName="Table1" ref="A1:C24" totalsRowShown="0">
+  <autoFilter ref="A1:C24" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -572,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44E78C7-E25B-460C-937F-CCE8B1E2A7B2}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +626,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -609,7 +637,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -620,194 +648,218 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>41</v>
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
-        <v>50</v>
+      <c r="A20" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>51</v>
       </c>
-      <c r="B21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
+      <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12/20 - Fan mount, LED channel, and wiring stuff
- Finished all crimps but ABL.
- Started mapping headers and began Wiki with corresponding article.
- Tested limit switches, fans, thermistors, bed heat, and finally first hotend heat and filament extrusion.
- Designed mount for programmable LEDs. Design is parametric based on spacing, PCB width, and LED count. Includes a zip tie anchor.
- LED tests. SP901E is finicky with WS2815, leaving it out for now.
- Nearly all connectors are now labeled.
- Resolved display issue.
- Added a modification of an old PTFE tubing coupler design. This part should go away in later revisions.
- First print should be tomorrow.
</commit_message>
<xml_diff>
--- a/Docs/Connectors.xlsx
+++ b/Docs/Connectors.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91143369-5505-4124-B5FE-F8637260D940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C743501C-7370-4915-A49D-B410626C5627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24288" yWindow="1296" windowWidth="26832" windowHeight="14196" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
+    <workbookView xWindow="10332" yWindow="5100" windowWidth="27792" windowHeight="13200" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
   <si>
     <t>Connector</t>
   </si>
@@ -79,9 +78,6 @@
     <t>Extruder Stepper</t>
   </si>
   <si>
-    <t>E0 (MOT4 on Octopus)</t>
-  </si>
-  <si>
     <t>X Limit Switch</t>
   </si>
   <si>
@@ -106,27 +102,6 @@
     <t>E0-DET/Z-MAX</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>LED Strip 1</t>
-  </si>
-  <si>
-    <t>LED Strip 2</t>
-  </si>
-  <si>
-    <t>LED Strip 3</t>
-  </si>
-  <si>
-    <t>Connects to splitter</t>
-  </si>
-  <si>
     <t>HB</t>
   </si>
   <si>
@@ -136,33 +111,18 @@
     <t>Bed Thermistor</t>
   </si>
   <si>
-    <t>External Connectors</t>
-  </si>
-  <si>
     <t>Alpha Stepper</t>
   </si>
   <si>
-    <t>X-MOT</t>
-  </si>
-  <si>
     <t>Beta Stepper</t>
   </si>
   <si>
-    <t>Y-MOT</t>
-  </si>
-  <si>
     <t>Z1 Stepper</t>
   </si>
   <si>
-    <t>Z-MOT</t>
-  </si>
-  <si>
     <t>Z2 Stepper</t>
   </si>
   <si>
-    <t>E1-MOT</t>
-  </si>
-  <si>
     <t>SX</t>
   </si>
   <si>
@@ -224,6 +184,96 @@
   </si>
   <si>
     <t>FH2</t>
+  </si>
+  <si>
+    <t>PSU</t>
+  </si>
+  <si>
+    <t>Power Supply</t>
+  </si>
+  <si>
+    <t>RPI</t>
+  </si>
+  <si>
+    <t>Raspberry Pi</t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>Electronics Thermistor</t>
+  </si>
+  <si>
+    <t>Fans</t>
+  </si>
+  <si>
+    <t>Lights</t>
+  </si>
+  <si>
+    <t>TH1</t>
+  </si>
+  <si>
+    <t>TH2</t>
+  </si>
+  <si>
+    <t>Thermistors</t>
+  </si>
+  <si>
+    <t>Limit Switches</t>
+  </si>
+  <si>
+    <t>MOT0</t>
+  </si>
+  <si>
+    <t>MOT1</t>
+  </si>
+  <si>
+    <t>MOT2-1</t>
+  </si>
+  <si>
+    <t>MOT3</t>
+  </si>
+  <si>
+    <t>MOT4</t>
+  </si>
+  <si>
+    <t>Steppers</t>
+  </si>
+  <si>
+    <t>FE1</t>
+  </si>
+  <si>
+    <t>Intake Fane</t>
+  </si>
+  <si>
+    <t>FAN1</t>
+  </si>
+  <si>
+    <t>FAN4</t>
+  </si>
+  <si>
+    <t>FE2</t>
+  </si>
+  <si>
+    <t>Exhaust Fan</t>
+  </si>
+  <si>
+    <t>FAN3</t>
+  </si>
+  <si>
+    <t>FAN6</t>
+  </si>
+  <si>
+    <t>FE3</t>
+  </si>
+  <si>
+    <t>LGT</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Stepper Driver Fan</t>
   </si>
 </sst>
 </file>
@@ -288,8 +338,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}" name="Table1" displayName="Table1" ref="A1:C24" totalsRowShown="0">
-  <autoFilter ref="A1:C24" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0">
+  <autoFilter ref="A1:C32" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -600,16 +650,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44E78C7-E25B-460C-937F-CCE8B1E2A7B2}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -625,47 +675,41 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="A2" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -681,185 +725,258 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
+      <c r="A9" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
+      <c r="A14" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" t="s">
-        <v>60</v>
+      <c r="A19" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
01/04 - 01/06 Wiring and skirt work
See changelog.md. Lots of quick changes to the panel mounts and general connector work.
</commit_message>
<xml_diff>
--- a/Docs/Connectors.xlsx
+++ b/Docs/Connectors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C743501C-7370-4915-A49D-B410626C5627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C08EFC-069A-470C-B348-2113E4B60AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10332" yWindow="5100" windowWidth="27792" windowHeight="13200" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
+    <workbookView xWindow="24120" yWindow="564" windowWidth="18444" windowHeight="13200" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="80">
-  <si>
-    <t>Connector</t>
-  </si>
-  <si>
-    <t>Terminal Label</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="97">
   <si>
     <t>Short Name</t>
   </si>
@@ -87,21 +81,9 @@
     <t>Left Z Limit Switch</t>
   </si>
   <si>
-    <t>Y-STOP/Y-MIN</t>
-  </si>
-  <si>
-    <t>X-STOP/X-MIN</t>
-  </si>
-  <si>
-    <t>Z-STOP/Z-MIN</t>
-  </si>
-  <si>
     <t>Right Z Limit Switch</t>
   </si>
   <si>
-    <t>E0-DET/Z-MAX</t>
-  </si>
-  <si>
     <t>HB</t>
   </si>
   <si>
@@ -111,18 +93,6 @@
     <t>Bed Thermistor</t>
   </si>
   <si>
-    <t>Alpha Stepper</t>
-  </si>
-  <si>
-    <t>Beta Stepper</t>
-  </si>
-  <si>
-    <t>Z1 Stepper</t>
-  </si>
-  <si>
-    <t>Z2 Stepper</t>
-  </si>
-  <si>
     <t>SX</t>
   </si>
   <si>
@@ -243,9 +213,6 @@
     <t>FE1</t>
   </si>
   <si>
-    <t>Intake Fane</t>
-  </si>
-  <si>
     <t>FAN1</t>
   </si>
   <si>
@@ -274,6 +241,90 @@
   </si>
   <si>
     <t>Stepper Driver Fan</t>
+  </si>
+  <si>
+    <t>Z1 (Left) Stepper</t>
+  </si>
+  <si>
+    <t>Z2 (Right) Stepper</t>
+  </si>
+  <si>
+    <t>Alpha (Left) Stepper</t>
+  </si>
+  <si>
+    <t>Beta (Right) Stepper</t>
+  </si>
+  <si>
+    <t>FAN5</t>
+  </si>
+  <si>
+    <t>HE3</t>
+  </si>
+  <si>
+    <t>HE2</t>
+  </si>
+  <si>
+    <t>FE4</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>24V</t>
+  </si>
+  <si>
+    <t>12V</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>Suppy Voltage</t>
+  </si>
+  <si>
+    <t>Intake Fan 1</t>
+  </si>
+  <si>
+    <t>Intake Fan 2</t>
+  </si>
+  <si>
+    <t>Varies Regionally</t>
+  </si>
+  <si>
+    <t>FAN7</t>
+  </si>
+  <si>
+    <t>5V (NC)</t>
+  </si>
+  <si>
+    <t>12V (NC)</t>
+  </si>
+  <si>
+    <t>Lights, secondary</t>
+  </si>
+  <si>
+    <t>STOP3</t>
+  </si>
+  <si>
+    <t>STOP2</t>
+  </si>
+  <si>
+    <t>STOP1</t>
+  </si>
+  <si>
+    <t>STOP0</t>
+  </si>
+  <si>
+    <t>Octopus Header Label</t>
+  </si>
+  <si>
+    <t>Lights, Signal</t>
+  </si>
+  <si>
+    <t>STOP-4</t>
+  </si>
+  <si>
+    <t>BLTouch</t>
   </si>
 </sst>
 </file>
@@ -338,16 +389,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0">
-  <autoFilter ref="A1:C32" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}" name="Table1" displayName="Table1" ref="A1:D35" totalsRowShown="0">
+  <autoFilter ref="A1:D35" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="3">
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D3612DE8-6536-466E-A137-4993F20AC6EE}" name="Short Name"/>
-    <tableColumn id="2" xr3:uid="{6F2ADC15-AB84-4A69-8025-B7142F348015}" name="Connector"/>
-    <tableColumn id="3" xr3:uid="{0CD11C45-8D63-4F31-9A69-974AAF728591}" name="Terminal Label"/>
+    <tableColumn id="2" xr3:uid="{6F2ADC15-AB84-4A69-8025-B7142F348015}" name="Component"/>
+    <tableColumn id="4" xr3:uid="{532E2B48-44FD-478A-A60E-F10CC10FA11F}" name="Suppy Voltage"/>
+    <tableColumn id="3" xr3:uid="{0CD11C45-8D63-4F31-9A69-974AAF728591}" name="Octopus Header Label"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -650,333 +703,430 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44E78C7-E25B-460C-937F-CCE8B1E2A7B2}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" t="s">
-        <v>46</v>
-      </c>
-      <c r="C28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
01/08 - Added SD Card mount
</commit_message>
<xml_diff>
--- a/Docs/Connectors.xlsx
+++ b/Docs/Connectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C08EFC-069A-470C-B348-2113E4B60AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F1798F-90C3-4957-B9C3-90A7740494E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24120" yWindow="564" windowWidth="18444" windowHeight="13200" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
   <si>
     <t>Short Name</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Hotend Thermistor</t>
   </si>
   <si>
-    <t>TH0</t>
-  </si>
-  <si>
     <t>Part Cooling Fan</t>
   </si>
   <si>
@@ -156,12 +153,6 @@
     <t>FH2</t>
   </si>
   <si>
-    <t>PSU</t>
-  </si>
-  <si>
-    <t>Power Supply</t>
-  </si>
-  <si>
     <t>RPI</t>
   </si>
   <si>
@@ -180,12 +171,6 @@
     <t>Lights</t>
   </si>
   <si>
-    <t>TH1</t>
-  </si>
-  <si>
-    <t>TH2</t>
-  </si>
-  <si>
     <t>Thermistors</t>
   </si>
   <si>
@@ -258,7 +243,7 @@
     <t>FAN5</t>
   </si>
   <si>
-    <t>HE3</t>
+    <t>HE1</t>
   </si>
   <si>
     <t>HE2</t>
@@ -288,9 +273,6 @@
     <t>Intake Fan 2</t>
   </si>
   <si>
-    <t>Varies Regionally</t>
-  </si>
-  <si>
     <t>FAN7</t>
   </si>
   <si>
@@ -321,10 +303,19 @@
     <t>Lights, Signal</t>
   </si>
   <si>
-    <t>STOP-4</t>
-  </si>
-  <si>
     <t>BLTouch</t>
+  </si>
+  <si>
+    <t>STOP4</t>
+  </si>
+  <si>
+    <t>T0</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
   </si>
 </sst>
 </file>
@@ -389,8 +380,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}" name="Table1" displayName="Table1" ref="A1:D35" totalsRowShown="0">
-  <autoFilter ref="A1:D35" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}" name="Table1" displayName="Table1" ref="A1:D34" totalsRowShown="0">
+  <autoFilter ref="A1:D34" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -703,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44E78C7-E25B-460C-937F-CCE8B1E2A7B2}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,29 +713,29 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -752,99 +743,99 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
         <v>79</v>
-      </c>
-      <c r="D6" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="A10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -854,11 +845,8 @@
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>80</v>
-      </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -868,11 +856,8 @@
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
-        <v>80</v>
-      </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -882,139 +867,136 @@
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
-        <v>80</v>
-      </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" t="s">
-        <v>89</v>
+      <c r="A15" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>50</v>
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
+      <c r="A20" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>57</v>
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" t="s">
-        <v>56</v>
+      <c r="A26" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>46</v>
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1022,27 +1004,27 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1053,80 +1035,66 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM and model updates
## 2022-02-15

- Fixed a ton of minor issues with brackets in the model.
- All brackets are now properly positioned and should be propogated.
- Removed brackets from the bed frame; will rely solely on printed parts.
- Bracket assemblies still used SHCS instead of button head; fixed and propagated.
- Filtration is in the model.
- Finished renaming printed part numbers.
- SP901E has a placeholder body with fasteners in the model, temporarily addressing #21 .

## 2022-02-14

- Fixed outer frame for part ID purposes.
- Added invisible SP901E assembly to the model to get it and the appropriate fasteners inventoried.
- Updated base foot and LED strips for part numbers.
- Too many minor changes to count.
- Lots of work on the prototype to reassemble the fixed skirt panels.
</commit_message>
<xml_diff>
--- a/Docs/Connectors.xlsx
+++ b/Docs/Connectors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6535E8E-099C-490B-A278-31919A5349F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE63477-F7D8-45A1-8D42-C538F5702696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="92">
   <si>
     <t>Short Name</t>
   </si>
@@ -201,9 +201,6 @@
     <t>FAN1</t>
   </si>
   <si>
-    <t>FAN4</t>
-  </si>
-  <si>
     <t>FE2</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>General</t>
   </si>
   <si>
-    <t>Stepper Driver Fan</t>
-  </si>
-  <si>
     <t>Z1 (Left) Stepper</t>
   </si>
   <si>
@@ -247,9 +241,6 @@
   </si>
   <si>
     <t>HE2</t>
-  </si>
-  <si>
-    <t>FE4</t>
   </si>
   <si>
     <t>Component</t>
@@ -383,8 +374,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}" name="Table1" displayName="Table1" ref="A1:D34" totalsRowShown="0">
-  <autoFilter ref="A1:D34" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0">
+  <autoFilter ref="A1:D33" xr:uid="{81D963E9-CE95-4BC2-948A-F06F71DA6788}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -697,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44E78C7-E25B-460C-937F-CCE8B1E2A7B2}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,18 +707,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -738,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -752,7 +743,7 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -760,44 +751,44 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -808,10 +799,10 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -822,7 +813,7 @@
         <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -838,7 +829,7 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -849,7 +840,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -860,7 +851,7 @@
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -871,7 +862,7 @@
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -898,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -909,7 +900,7 @@
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -920,7 +911,7 @@
         <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -933,7 +924,7 @@
         <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
         <v>47</v>
@@ -944,7 +935,7 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
         <v>48</v>
@@ -955,7 +946,7 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
         <v>49</v>
@@ -966,7 +957,7 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
         <v>50</v>
@@ -996,7 +987,7 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -1010,7 +1001,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
         <v>54</v>
@@ -1024,10 +1015,10 @@
         <v>35</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,10 +1029,10 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1049,24 +1040,24 @@
         <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
         <v>56</v>
       </c>
-      <c r="B32" t="s">
-        <v>57</v>
-      </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D32" t="s">
         <v>5</v>
@@ -1074,30 +1065,16 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" t="s">
-        <v>63</v>
-      </c>
-      <c r="C34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Parts, connectors, and minor fixes
## 2022-02-22

- Adjusted PN083/PN084 clearances around the extrusion.
- Tweaking master part list entries a bit, adding "Supplies" category that includes items of indeterminate quantity (e.g. lubricant) or that may be on hand as a tool (e.g. screwdrivers) and generally don't go on a BOM but will be needed.
- Removed old PN082 file.
- Rebalanced screws on the Z Gantries. There are now three M5 on top, three under.
- Finished insulation and fasteners for all of the panels but the flooring.
- Updated the master model and removed old paneling.
- Added in feet to the `Outer Frame` model.

## 2022-02-21

- Turns out PN083 and PN084's issues are not thickness underneath the insert but severe ringing by the printer. Removed the issue. Will fix belt tension on printer later.
- Adding insulation and joints to the new panel models in the Outer Frame file.
- Finishing out the connector list based on the wire harnesses.
</commit_message>
<xml_diff>
--- a/Docs/Connectors.xlsx
+++ b/Docs/Connectors.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E15ED80-44B6-4F96-85C3-AA8AE6952B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF39A7F9-72A0-4118-9AD2-E67E1DB306B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28290" yWindow="2370" windowWidth="23250" windowHeight="12480" activeTab="1" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
+    <workbookView xWindow="-27945" yWindow="2715" windowWidth="23250" windowHeight="12480" activeTab="1" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Connector IDs" sheetId="1" r:id="rId1"/>
     <sheet name="Upper Level Wiring" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="121">
   <si>
     <t>Short Name</t>
   </si>
@@ -371,6 +372,33 @@
   </si>
   <si>
     <t>Back Lights</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Z1 Limit Switch</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>WKYRG</t>
+  </si>
+  <si>
+    <t>1/2" PET wire loom</t>
+  </si>
+  <si>
+    <t>1/4" PET wire loom</t>
+  </si>
+  <si>
+    <t>WW</t>
+  </si>
+  <si>
+    <t>RGK</t>
+  </si>
+  <si>
+    <t>4mm OD/2mm ID PTFE</t>
   </si>
 </sst>
 </file>
@@ -482,8 +510,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0354E98D-3659-45E4-8C0A-CE5AE43F1A3E}" name="Table13" displayName="Table13" ref="A1:F12" totalsRowShown="0">
-  <autoFilter ref="A1:F12" xr:uid="{DC48BFC0-82F8-4E68-A85C-1DBDC70C7484}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0354E98D-3659-45E4-8C0A-CE5AE43F1A3E}" name="Table13" displayName="Table13" ref="A1:F14" totalsRowShown="0">
+  <autoFilter ref="A1:F14" xr:uid="{DC48BFC0-82F8-4E68-A85C-1DBDC70C7484}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1215,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C1868B-6555-4CF5-BEB3-756D16E536C2}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,6 +1309,9 @@
       <c r="D3">
         <v>150</v>
       </c>
+      <c r="E3" t="s">
+        <v>118</v>
+      </c>
       <c r="F3" t="s">
         <v>93</v>
       </c>
@@ -1338,6 +1369,9 @@
       <c r="D6">
         <v>150</v>
       </c>
+      <c r="E6" t="s">
+        <v>115</v>
+      </c>
       <c r="F6" t="s">
         <v>84</v>
       </c>
@@ -1408,7 +1442,9 @@
       <c r="D10" s="2">
         <v>80</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>110</v>
       </c>
@@ -1443,12 +1479,103 @@
       <c r="D12">
         <v>110</v>
       </c>
+      <c r="E12" t="s">
+        <v>119</v>
+      </c>
       <c r="F12" t="s">
         <v>111</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>75</v>
+      </c>
+      <c r="F13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>80</v>
+      </c>
+      <c r="E14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>65</v>
+      </c>
+      <c r="F16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>90</v>
+      </c>
+      <c r="F18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>50</v>
+      </c>
+      <c r="F20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>50</v>
+      </c>
+      <c r="F21" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="B13" numberStoredAsText="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>

<commit_message>
Initial Panel STEP files
</commit_message>
<xml_diff>
--- a/Docs/Connectors.xlsx
+++ b/Docs/Connectors.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF39A7F9-72A0-4118-9AD2-E67E1DB306B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEDCDFA-29F7-4608-885A-61FF012E5F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27945" yWindow="2715" windowWidth="23250" windowHeight="12480" activeTab="1" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Connector IDs" sheetId="1" r:id="rId1"/>
     <sheet name="Upper Level Wiring" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="127">
   <si>
     <t>Short Name</t>
   </si>
@@ -399,6 +399,24 @@
   </si>
   <si>
     <t>4mm OD/2mm ID PTFE</t>
+  </si>
+  <si>
+    <t>Wrap</t>
+  </si>
+  <si>
+    <t>Conn B</t>
+  </si>
+  <si>
+    <t>Conn A</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Pin Count</t>
+  </si>
+  <si>
+    <t>Cable</t>
   </si>
 </sst>
 </file>
@@ -1245,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C1868B-6555-4CF5-BEB3-756D16E536C2}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,4 +1598,49 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220CAEEC-A537-49E7-8CB6-74590B623C46}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Wire and connector count update, BOM script improvements
- Tallied and labeled all wires, connectors, and pins.
- Updated ExtractBOM_PN. File location is currently hardcoded and it lacks a UI, but those are already on the radar.
</commit_message>
<xml_diff>
--- a/Docs/Connectors.xlsx
+++ b/Docs/Connectors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ACC041-94C0-404D-9E34-BFFAC046874C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC2058E-D2AD-43D6-8871-7E066D5E7EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
+    <workbookView xWindow="2730" yWindow="2595" windowWidth="13320" windowHeight="8985" activeTab="1" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Connector IDs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="208">
   <si>
     <t>Short Name</t>
   </si>
@@ -569,9 +569,6 @@
     <t>TE-A</t>
   </si>
   <si>
-    <t>SX F</t>
-  </si>
-  <si>
     <t>Soldered-on pigtail</t>
   </si>
   <si>
@@ -621,9 +618,6 @@
   </si>
   <si>
     <t>USB</t>
-  </si>
-  <si>
-    <t>Tot Len</t>
   </si>
   <si>
     <t>Part ID</t>
@@ -718,11 +712,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -754,12 +744,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DCEE01FF-B217-412A-8334-832E426EC070}" name="Table3" displayName="Table3" ref="A1:I55" totalsRowShown="0">
-  <autoFilter ref="A1:I55" xr:uid="{DCEE01FF-B217-412A-8334-832E426EC070}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DCEE01FF-B217-412A-8334-832E426EC070}" name="Table3" displayName="Table3" ref="A1:H55" totalsRowShown="0">
+  <autoFilter ref="A1:H55" xr:uid="{DCEE01FF-B217-412A-8334-832E426EC070}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H55">
     <sortCondition ref="C1:C55"/>
   </sortState>
-  <tableColumns count="9">
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{FBF2E2EC-CB79-4DAF-A0AD-5C50EC7D1CF7}" name="Cable"/>
     <tableColumn id="2" xr3:uid="{0DCCB1C4-6A24-4706-96E7-F2E992D16F07}" name="Component"/>
     <tableColumn id="3" xr3:uid="{12F9C25F-8EE1-4903-9829-BB393B754AE2}" name="AWG"/>
@@ -768,9 +758,6 @@
     <tableColumn id="6" xr3:uid="{41A61DCB-EB69-4ABD-AC8C-6A79DAAE3294}" name="Conn A"/>
     <tableColumn id="7" xr3:uid="{1D8EF2F9-8563-42CE-9B38-42AA63B17702}" name="Conn B"/>
     <tableColumn id="8" xr3:uid="{0634F095-E2EE-44F0-B066-066F504AA291}" name="Notes"/>
-    <tableColumn id="9" xr3:uid="{3019ADCC-9D4D-4BE2-8202-480C595FD971}" name="Tot Len" dataDxfId="0">
-      <calculatedColumnFormula>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</calculatedColumnFormula>
-    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1493,7 +1480,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1501,10 +1488,10 @@
         <v>151</v>
       </c>
       <c r="B35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C35" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1512,7 +1499,7 @@
         <v>158</v>
       </c>
       <c r="B36" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C36" t="s">
         <v>70</v>
@@ -1523,7 +1510,7 @@
         <v>167</v>
       </c>
       <c r="B37" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -1537,10 +1524,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220CAEEC-A537-49E7-8CB6-74590B623C46}">
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,7 +1541,7 @@
     <col min="8" max="8" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>101</v>
       </c>
@@ -1579,11 +1566,8 @@
       <c r="H1" t="s">
         <v>102</v>
       </c>
-      <c r="I1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>150</v>
       </c>
@@ -1608,12 +1592,8 @@
       <c r="H2" t="s">
         <v>154</v>
       </c>
-      <c r="I2">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -1638,12 +1618,8 @@
       <c r="H3" t="s">
         <v>156</v>
       </c>
-      <c r="I3">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>175</v>
       </c>
@@ -1668,12 +1644,8 @@
       <c r="H4" t="s">
         <v>155</v>
       </c>
-      <c r="I4">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>157</v>
       </c>
@@ -1698,12 +1670,8 @@
       <c r="H5" t="s">
         <v>159</v>
       </c>
-      <c r="I5">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>160</v>
       </c>
@@ -1728,12 +1696,8 @@
       <c r="H6" t="s">
         <v>161</v>
       </c>
-      <c r="I6">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -1758,12 +1722,8 @@
       <c r="H7" t="s">
         <v>162</v>
       </c>
-      <c r="I7">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -1788,12 +1748,8 @@
       <c r="H8" t="s">
         <v>168</v>
       </c>
-      <c r="I8">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>103</v>
       </c>
@@ -1815,12 +1771,8 @@
       <c r="G9" t="s">
         <v>118</v>
       </c>
-      <c r="I9">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>104</v>
       </c>
@@ -1842,12 +1794,8 @@
       <c r="G10" t="s">
         <v>118</v>
       </c>
-      <c r="I10">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>163</v>
       </c>
@@ -1872,12 +1820,8 @@
       <c r="H11" t="s">
         <v>165</v>
       </c>
-      <c r="I11">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>169</v>
       </c>
@@ -1902,12 +1846,8 @@
       <c r="H12" t="s">
         <v>170</v>
       </c>
-      <c r="I12">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -1929,12 +1869,8 @@
       <c r="G13" t="s">
         <v>118</v>
       </c>
-      <c r="I13">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -1956,12 +1892,8 @@
       <c r="G14" t="s">
         <v>118</v>
       </c>
-      <c r="I14">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>121</v>
       </c>
@@ -1983,12 +1915,8 @@
       <c r="G15" t="s">
         <v>118</v>
       </c>
-      <c r="I15">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -2010,12 +1938,8 @@
       <c r="G16" t="s">
         <v>118</v>
       </c>
-      <c r="I16">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>134</v>
       </c>
@@ -2037,12 +1961,8 @@
       <c r="G17" t="s">
         <v>118</v>
       </c>
-      <c r="I17">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>105</v>
       </c>
@@ -2064,12 +1984,8 @@
       <c r="G18" t="s">
         <v>118</v>
       </c>
-      <c r="I18">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>122</v>
       </c>
@@ -2092,14 +2008,10 @@
         <v>118</v>
       </c>
       <c r="H19" t="s">
-        <v>185</v>
-      </c>
-      <c r="I19">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>108</v>
       </c>
@@ -2121,12 +2033,8 @@
       <c r="G20" t="s">
         <v>118</v>
       </c>
-      <c r="I20">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>750</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>124</v>
       </c>
@@ -2148,12 +2056,8 @@
       <c r="G21" t="s">
         <v>118</v>
       </c>
-      <c r="I21">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -2175,12 +2079,8 @@
       <c r="G22" t="s">
         <v>118</v>
       </c>
-      <c r="I22">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>126</v>
       </c>
@@ -2205,12 +2105,8 @@
       <c r="H23" t="s">
         <v>127</v>
       </c>
-      <c r="I23">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -2232,12 +2128,8 @@
       <c r="G24" t="s">
         <v>118</v>
       </c>
-      <c r="I24">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>116</v>
       </c>
@@ -2259,12 +2151,8 @@
       <c r="G25" t="s">
         <v>118</v>
       </c>
-      <c r="I25">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>129</v>
       </c>
@@ -2287,14 +2175,10 @@
         <v>145</v>
       </c>
       <c r="H26" t="s">
-        <v>178</v>
-      </c>
-      <c r="I26">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -2316,12 +2200,8 @@
       <c r="G27" t="s">
         <v>118</v>
       </c>
-      <c r="I27">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>112</v>
       </c>
@@ -2343,12 +2223,8 @@
       <c r="G28" t="s">
         <v>118</v>
       </c>
-      <c r="I28">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>131</v>
       </c>
@@ -2371,14 +2247,10 @@
         <v>145</v>
       </c>
       <c r="H29" t="s">
-        <v>178</v>
-      </c>
-      <c r="I29">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>132</v>
       </c>
@@ -2401,14 +2273,10 @@
         <v>118</v>
       </c>
       <c r="H30" t="s">
-        <v>184</v>
-      </c>
-      <c r="I30">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2430,12 +2298,8 @@
       <c r="G31" t="s">
         <v>118</v>
       </c>
-      <c r="I31">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>133</v>
       </c>
@@ -2458,14 +2322,10 @@
         <v>145</v>
       </c>
       <c r="H32" t="s">
-        <v>178</v>
-      </c>
-      <c r="I32">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>135</v>
       </c>
@@ -2487,12 +2347,8 @@
       <c r="G33" t="s">
         <v>118</v>
       </c>
-      <c r="I33">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -2512,14 +2368,10 @@
         <v>119</v>
       </c>
       <c r="G34" t="s">
-        <v>177</v>
-      </c>
-      <c r="I34">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>270</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -2541,12 +2393,8 @@
       <c r="G35" t="s">
         <v>118</v>
       </c>
-      <c r="I35">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>113</v>
       </c>
@@ -2566,14 +2414,10 @@
         <v>119</v>
       </c>
       <c r="G36" t="s">
-        <v>177</v>
-      </c>
-      <c r="I36">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>315</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>137</v>
       </c>
@@ -2595,12 +2439,8 @@
       <c r="G37" t="s">
         <v>118</v>
       </c>
-      <c r="I37">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>195</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>115</v>
       </c>
@@ -2620,14 +2460,10 @@
         <v>119</v>
       </c>
       <c r="G38" t="s">
-        <v>177</v>
-      </c>
-      <c r="I38">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>225</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>138</v>
       </c>
@@ -2649,12 +2485,8 @@
       <c r="G39" t="s">
         <v>118</v>
       </c>
-      <c r="I39">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>111</v>
       </c>
@@ -2674,14 +2506,10 @@
         <v>119</v>
       </c>
       <c r="G40" t="s">
-        <v>177</v>
-      </c>
-      <c r="I40">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>225</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>141</v>
       </c>
@@ -2703,12 +2531,8 @@
       <c r="G41" t="s">
         <v>118</v>
       </c>
-      <c r="I41">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>280</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>142</v>
       </c>
@@ -2728,14 +2552,10 @@
         <v>118</v>
       </c>
       <c r="H42" t="s">
-        <v>179</v>
-      </c>
-      <c r="I42">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>143</v>
       </c>
@@ -2757,12 +2577,8 @@
       <c r="G43" t="s">
         <v>118</v>
       </c>
-      <c r="I43">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>280</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>144</v>
       </c>
@@ -2785,14 +2601,10 @@
         <v>118</v>
       </c>
       <c r="H44" t="s">
-        <v>179</v>
-      </c>
-      <c r="I44">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>400</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>139</v>
       </c>
@@ -2817,12 +2629,8 @@
       <c r="H45" t="s">
         <v>127</v>
       </c>
-      <c r="I45">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>140</v>
       </c>
@@ -2847,12 +2655,8 @@
       <c r="H46" t="s">
         <v>127</v>
       </c>
-      <c r="I46">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>171</v>
       </c>
@@ -2874,12 +2678,8 @@
       <c r="G47" t="s">
         <v>118</v>
       </c>
-      <c r="I47">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>172</v>
       </c>
@@ -2901,12 +2701,8 @@
       <c r="G48" t="s">
         <v>118</v>
       </c>
-      <c r="I48">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>173</v>
       </c>
@@ -2928,12 +2724,8 @@
       <c r="G49" t="s">
         <v>118</v>
       </c>
-      <c r="I49">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>176</v>
       </c>
@@ -2955,14 +2747,10 @@
       <c r="G50" t="s">
         <v>118</v>
       </c>
-      <c r="I50">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B51" t="s">
         <v>33</v>
@@ -2982,14 +2770,10 @@
       <c r="G51" t="s">
         <v>118</v>
       </c>
-      <c r="I51">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B52" t="s">
         <v>33</v>
@@ -3009,14 +2793,10 @@
       <c r="G52" t="s">
         <v>118</v>
       </c>
-      <c r="I52">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B53" t="s">
         <v>33</v>
@@ -3036,14 +2816,10 @@
       <c r="G53" t="s">
         <v>118</v>
       </c>
-      <c r="I53">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B54" t="s">
         <v>33</v>
@@ -3063,12 +2839,8 @@
       <c r="G54" t="s">
         <v>118</v>
       </c>
-      <c r="I54">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>123</v>
       </c>
@@ -3092,10 +2864,6 @@
       </c>
       <c r="H55" t="s">
         <v>125</v>
-      </c>
-      <c r="I55">
-        <f>Table3[[#This Row],[Pin Count]]*Table3[[#This Row],[Len (cm)]]</f>
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3110,7 +2878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E4094C-9254-4EC7-8CD2-E477AEAD8BCF}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -3123,10 +2891,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C1" t="s">
         <v>90</v>
@@ -3140,47 +2908,47 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" t="s">
         <v>187</v>
-      </c>
-      <c r="C3" t="s">
-        <v>188</v>
       </c>
       <c r="D3">
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D4">
         <v>100</v>
@@ -3188,36 +2956,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C5" t="s">
         <v>191</v>
-      </c>
-      <c r="C5" t="s">
-        <v>192</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D6">
         <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bill of materials/part list updates
Lots of fixes today required re-exporting the part list and regenerating the BOM.
</commit_message>
<xml_diff>
--- a/Docs/Connectors.xlsx
+++ b/Docs/Connectors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC2058E-D2AD-43D6-8871-7E066D5E7EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE908B9-4BD2-42C0-A0DB-C0228007B1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2595" windowWidth="13320" windowHeight="8985" activeTab="1" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
+    <workbookView xWindow="-19950" yWindow="1245" windowWidth="15330" windowHeight="14535" activeTab="1" xr2:uid="{2BA3904D-48D5-4484-9C88-BD860323DFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Connector IDs" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="223">
   <si>
     <t>Short Name</t>
   </si>
@@ -392,9 +392,6 @@
     <t>Len (cm)</t>
   </si>
   <si>
-    <t>SM F</t>
-  </si>
-  <si>
     <t>SM M</t>
   </si>
   <si>
@@ -479,12 +476,6 @@
     <t>XH F</t>
   </si>
   <si>
-    <t>JST-SH F</t>
-  </si>
-  <si>
-    <t>JST-PH F</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -660,6 +651,60 @@
   </si>
   <si>
     <t>For MCU &lt;-&gt; RPI comms</t>
+  </si>
+  <si>
+    <t>LGT-A1</t>
+  </si>
+  <si>
+    <t>Pairs with LGT-A2</t>
+  </si>
+  <si>
+    <t>LGT-A2</t>
+  </si>
+  <si>
+    <t>Pairs with LGT-A2, uses 3 pin connector</t>
+  </si>
+  <si>
+    <t>XH F3</t>
+  </si>
+  <si>
+    <t>XH F2</t>
+  </si>
+  <si>
+    <t>SM M5</t>
+  </si>
+  <si>
+    <t>SM M2</t>
+  </si>
+  <si>
+    <t>XH F4</t>
+  </si>
+  <si>
+    <t>SM M4</t>
+  </si>
+  <si>
+    <t>SM M3</t>
+  </si>
+  <si>
+    <t>JST-SH F5</t>
+  </si>
+  <si>
+    <t>SM F2</t>
+  </si>
+  <si>
+    <t>SM F5</t>
+  </si>
+  <si>
+    <t>SM F4</t>
+  </si>
+  <si>
+    <t>JST-PH F4</t>
+  </si>
+  <si>
+    <t>SM F3</t>
+  </si>
+  <si>
+    <t>LGT-A3</t>
   </si>
 </sst>
 </file>
@@ -744,8 +789,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DCEE01FF-B217-412A-8334-832E426EC070}" name="Table3" displayName="Table3" ref="A1:H55" totalsRowShown="0">
-  <autoFilter ref="A1:H55" xr:uid="{DCEE01FF-B217-412A-8334-832E426EC070}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DCEE01FF-B217-412A-8334-832E426EC070}" name="Table3" displayName="Table3" ref="A1:H58" totalsRowShown="0">
+  <autoFilter ref="A1:H58" xr:uid="{DCEE01FF-B217-412A-8334-832E426EC070}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H55">
     <sortCondition ref="C1:C55"/>
   </sortState>
@@ -1077,7 +1122,7 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1480,26 +1525,26 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B35" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C35" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B36" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C36" t="s">
         <v>70</v>
@@ -1507,10 +1552,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B37" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1524,10 +1569,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220CAEEC-A537-49E7-8CB6-74590B623C46}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1583,7 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1569,10 +1614,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C2">
         <v>16</v>
@@ -1584,21 +1629,21 @@
         <v>80</v>
       </c>
       <c r="F2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C3">
         <v>16</v>
@@ -1610,21 +1655,21 @@
         <v>75</v>
       </c>
       <c r="F3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G3" t="s">
+        <v>150</v>
+      </c>
+      <c r="H3" t="s">
         <v>153</v>
-      </c>
-      <c r="H3" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -1636,21 +1681,21 @@
         <v>25</v>
       </c>
       <c r="F4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" t="s">
         <v>152</v>
-      </c>
-      <c r="G4" t="s">
-        <v>153</v>
-      </c>
-      <c r="H4" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -1662,21 +1707,21 @@
         <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -1688,21 +1733,21 @@
         <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -1714,21 +1759,21 @@
         <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1740,13 +1785,13 @@
         <v>25</v>
       </c>
       <c r="F8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1766,10 +1811,10 @@
         <v>55</v>
       </c>
       <c r="F9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G9" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1789,18 +1834,18 @@
         <v>150</v>
       </c>
       <c r="F10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G10" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C11">
         <v>22</v>
@@ -1812,21 +1857,21 @@
         <v>55</v>
       </c>
       <c r="F11" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C12">
         <v>22</v>
@@ -1838,18 +1883,18 @@
         <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -1864,10 +1909,10 @@
         <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>146</v>
+        <v>210</v>
       </c>
       <c r="G13" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1887,15 +1932,15 @@
         <v>150</v>
       </c>
       <c r="F14" t="s">
-        <v>119</v>
+        <v>212</v>
       </c>
       <c r="G14" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
@@ -1910,10 +1955,10 @@
         <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>146</v>
+        <v>210</v>
       </c>
       <c r="G15" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1933,15 +1978,15 @@
         <v>150</v>
       </c>
       <c r="F16" t="s">
-        <v>119</v>
+        <v>212</v>
       </c>
       <c r="G16" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
@@ -1956,10 +2001,10 @@
         <v>40</v>
       </c>
       <c r="F17" t="s">
-        <v>146</v>
+        <v>210</v>
       </c>
       <c r="G17" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1979,15 +2024,15 @@
         <v>150</v>
       </c>
       <c r="F18" t="s">
-        <v>119</v>
+        <v>212</v>
       </c>
       <c r="G18" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
@@ -2002,13 +2047,13 @@
         <v>40</v>
       </c>
       <c r="F19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
+        <v>218</v>
       </c>
       <c r="H19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2028,15 +2073,15 @@
         <v>150</v>
       </c>
       <c r="F20" t="s">
-        <v>119</v>
+        <v>211</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
         <v>30</v>
@@ -2051,10 +2096,10 @@
         <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="G21" t="s">
-        <v>118</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2074,15 +2119,15 @@
         <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>119</v>
+        <v>214</v>
       </c>
       <c r="G22" t="s">
-        <v>118</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
         <v>30</v>
@@ -2097,18 +2142,18 @@
         <v>5</v>
       </c>
       <c r="F23" t="s">
-        <v>119</v>
+        <v>214</v>
       </c>
       <c r="G23" t="s">
-        <v>148</v>
+        <v>220</v>
       </c>
       <c r="H23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s">
         <v>97</v>
@@ -2123,10 +2168,10 @@
         <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G24" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2146,15 +2191,15 @@
         <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="G25" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B26" t="s">
         <v>97</v>
@@ -2169,18 +2214,18 @@
         <v>5</v>
       </c>
       <c r="F26" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="G26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H26" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
         <v>93</v>
@@ -2195,10 +2240,10 @@
         <v>80</v>
       </c>
       <c r="F27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G27" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2218,15 +2263,15 @@
         <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="G28" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B29" t="s">
         <v>93</v>
@@ -2241,18 +2286,18 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="G29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H29" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B30" t="s">
         <v>92</v>
@@ -2267,13 +2312,13 @@
         <v>80</v>
       </c>
       <c r="F30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G30" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
       <c r="H30" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2293,15 +2338,15 @@
         <v>110</v>
       </c>
       <c r="F31" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="G31" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B32" t="s">
         <v>92</v>
@@ -2316,18 +2361,18 @@
         <v>5</v>
       </c>
       <c r="F32" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="G32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H32" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
@@ -2342,10 +2387,10 @@
         <v>35</v>
       </c>
       <c r="F33" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="G33" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2365,15 +2410,15 @@
         <v>90</v>
       </c>
       <c r="F34" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="G34" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B35" t="s">
         <v>19</v>
@@ -2388,10 +2433,10 @@
         <v>30</v>
       </c>
       <c r="F35" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="G35" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2411,15 +2456,15 @@
         <v>105</v>
       </c>
       <c r="F36" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="G36" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B37" t="s">
         <v>20</v>
@@ -2434,10 +2479,10 @@
         <v>65</v>
       </c>
       <c r="F37" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="G37" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2457,15 +2502,15 @@
         <v>75</v>
       </c>
       <c r="F38" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="G38" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B39" t="s">
         <v>21</v>
@@ -2480,10 +2525,10 @@
         <v>30</v>
       </c>
       <c r="F39" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="G39" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2503,15 +2548,15 @@
         <v>75</v>
       </c>
       <c r="F40" t="s">
-        <v>119</v>
+        <v>215</v>
       </c>
       <c r="G40" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B41" t="s">
         <v>29</v>
@@ -2526,15 +2571,15 @@
         <v>70</v>
       </c>
       <c r="F41" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="G41" t="s">
-        <v>118</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
@@ -2546,18 +2591,18 @@
         <v>4</v>
       </c>
       <c r="F42" t="s">
-        <v>119</v>
+        <v>214</v>
       </c>
       <c r="G42" t="s">
-        <v>118</v>
+        <v>219</v>
       </c>
       <c r="H42" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B43" t="s">
         <v>28</v>
@@ -2572,15 +2617,15 @@
         <v>70</v>
       </c>
       <c r="F43" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="G43" t="s">
-        <v>118</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B44" t="s">
         <v>28</v>
@@ -2595,18 +2640,18 @@
         <v>100</v>
       </c>
       <c r="F44" t="s">
-        <v>119</v>
+        <v>214</v>
       </c>
       <c r="G44" t="s">
-        <v>118</v>
+        <v>219</v>
       </c>
       <c r="H44" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B45" t="s">
         <v>27</v>
@@ -2621,18 +2666,18 @@
         <v>30</v>
       </c>
       <c r="F45" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="G45" t="s">
-        <v>148</v>
+        <v>220</v>
       </c>
       <c r="H45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B46" t="s">
         <v>26</v>
@@ -2647,18 +2692,18 @@
         <v>40</v>
       </c>
       <c r="F46" t="s">
-        <v>146</v>
+        <v>213</v>
       </c>
       <c r="G46" t="s">
-        <v>148</v>
+        <v>220</v>
       </c>
       <c r="H46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B47" t="s">
         <v>24</v>
@@ -2673,15 +2718,15 @@
         <v>60</v>
       </c>
       <c r="F47" t="s">
-        <v>146</v>
+        <v>210</v>
       </c>
       <c r="G47" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B48" t="s">
         <v>31</v>
@@ -2696,15 +2741,15 @@
         <v>60</v>
       </c>
       <c r="F48" t="s">
-        <v>146</v>
+        <v>210</v>
       </c>
       <c r="G48" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B49" t="s">
         <v>31</v>
@@ -2719,15 +2764,15 @@
         <v>35</v>
       </c>
       <c r="F49" t="s">
-        <v>119</v>
+        <v>212</v>
       </c>
       <c r="G49" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B50" t="s">
         <v>41</v>
@@ -2742,15 +2787,15 @@
         <v>35</v>
       </c>
       <c r="F50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G50" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B51" t="s">
         <v>33</v>
@@ -2765,15 +2810,15 @@
         <v>60</v>
       </c>
       <c r="F51" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G51" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B52" t="s">
         <v>33</v>
@@ -2788,15 +2833,15 @@
         <v>70</v>
       </c>
       <c r="F52" t="s">
-        <v>119</v>
+        <v>212</v>
       </c>
       <c r="G52" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B53" t="s">
         <v>33</v>
@@ -2811,15 +2856,15 @@
         <v>60</v>
       </c>
       <c r="F53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G53" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B54" t="s">
         <v>33</v>
@@ -2834,15 +2879,15 @@
         <v>70</v>
       </c>
       <c r="F54" t="s">
-        <v>119</v>
+        <v>212</v>
       </c>
       <c r="G54" t="s">
-        <v>118</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B55" t="s">
         <v>8</v>
@@ -2857,13 +2902,88 @@
         <v>6</v>
       </c>
       <c r="F55" t="s">
-        <v>119</v>
+        <v>211</v>
       </c>
       <c r="G55" t="s">
-        <v>147</v>
+        <v>216</v>
       </c>
       <c r="H55" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>205</v>
+      </c>
+      <c r="B56" t="s">
+        <v>60</v>
+      </c>
+      <c r="C56">
+        <v>24</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56">
+        <v>85</v>
+      </c>
+      <c r="F56" t="s">
+        <v>210</v>
+      </c>
+      <c r="G56" t="s">
+        <v>144</v>
+      </c>
+      <c r="H56" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>207</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57">
+        <v>24</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>85</v>
+      </c>
+      <c r="F57" t="s">
+        <v>209</v>
+      </c>
+      <c r="G57" t="s">
+        <v>144</v>
+      </c>
+      <c r="H57" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>222</v>
+      </c>
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58">
+        <v>24</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>85</v>
+      </c>
+      <c r="F58" t="s">
+        <v>210</v>
+      </c>
+      <c r="G58" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2891,10 +3011,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C1" t="s">
         <v>90</v>
@@ -2908,47 +3028,47 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D3">
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D4">
         <v>100</v>
@@ -2956,36 +3076,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D5">
         <v>100</v>
       </c>
       <c r="E5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D6">
         <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>